<commit_message>
updated files, source codes, model building and visualization
</commit_message>
<xml_diff>
--- a/Models Evaluation report.xlsx
+++ b/Models Evaluation report.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Seneca_DSA\4yr_Semester_8\Capstone Project BDC800NAA\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Seneca_DSA\4yr_Semester_8\Capstone Project BDC800NAA\Group Project\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218E5A19-FFB5-4C07-8A76-D1640082B25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4683E724-0FE7-4AE6-9287-4E78E29ABB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FFF3F5EE-C62B-44A0-809D-66B774E627B0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{FFF3F5EE-C62B-44A0-809D-66B774E627B0}"/>
   </bookViews>
   <sheets>
     <sheet name="17 Features" sheetId="2" r:id="rId1"/>
     <sheet name="13 Features" sheetId="3" r:id="rId2"/>
+    <sheet name="19 Features " sheetId="4" r:id="rId3"/>
+    <sheet name="19 Features  testing with Activ" sheetId="5" r:id="rId4"/>
+    <sheet name="19 Features - Final" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="28">
   <si>
     <t>Attempt</t>
   </si>
@@ -95,12 +98,39 @@
   <si>
     <t>Used All 17 Features</t>
   </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>Activation</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>Training Dataset</t>
+  </si>
+  <si>
+    <t>Testing Dataset</t>
+  </si>
+  <si>
+    <t>Used All 19 Features - Final Evaluation</t>
+  </si>
+  <si>
+    <t>Neural Network Model (# 10)</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +149,14 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -646,48 +684,215 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -710,17 +915,53 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,46 +975,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -787,6 +1010,156 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354126B5-F91B-48C9-90A7-F338DC9B6EB0}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1114,68 +1487,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="7">
         <v>0.76600000000000001</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="7">
         <v>0.80400000000000005</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="7">
         <v>0.70399999999999996</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="8">
         <v>0.751</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="1">
         <v>0.79800000000000004</v>
       </c>
@@ -1190,34 +1563,34 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15">
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="9">
         <v>0.79800000000000004</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="9">
         <v>0.85299999999999998</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="9">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="10">
         <v>0.78200000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="1">
         <v>0.79800000000000004</v>
       </c>
@@ -1232,120 +1605,120 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="11">
         <v>0.79800000000000004</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="11">
         <v>0.85399999999999998</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="11">
         <v>0.72</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="12">
         <v>0.78100000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="48" t="s">
+      <c r="H10" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="49" t="s">
+      <c r="I10" s="54" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="57"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="55"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="14">
         <v>10</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="15">
         <v>8</v>
       </c>
-      <c r="D12" s="24">
-        <v>1</v>
-      </c>
-      <c r="E12" s="25">
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17">
         <v>100</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="18">
         <v>0.76</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="15">
         <v>0.78300000000000003</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="15">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="16">
         <v>0.751</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
         <v>20</v>
       </c>
       <c r="C13" s="1">
@@ -1354,10 +1727,10 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>50</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <v>0.79800000000000004</v>
       </c>
       <c r="G13" s="1">
@@ -1371,39 +1744,39 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="19">
         <v>2</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="20">
         <v>20</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="9">
         <v>10</v>
       </c>
-      <c r="D14" s="16">
-        <v>1</v>
-      </c>
-      <c r="E14" s="29">
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21">
         <v>50</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="22">
         <v>0.79800000000000004</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="9">
         <v>0.85299999999999998</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="9">
         <v>0.72199999999999998</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="10">
         <v>0.78200000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>3</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <v>25</v>
       </c>
       <c r="C15" s="1">
@@ -1412,10 +1785,10 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>100</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="4">
         <v>0.79900000000000004</v>
       </c>
       <c r="G15" s="1">
@@ -1429,39 +1802,39 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="19">
         <v>4</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="20">
         <v>20</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="9">
         <v>6</v>
       </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="29">
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21">
         <v>50</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="22">
         <v>0.79700000000000004</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="9">
         <v>0.85499999999999998</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="10">
         <v>0.78</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="6">
         <v>5</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>20</v>
       </c>
       <c r="C17" s="1">
@@ -1470,10 +1843,10 @@
       <c r="D17" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>50</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="4">
         <v>0.79700000000000004</v>
       </c>
       <c r="G17" s="1">
@@ -1487,39 +1860,39 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="19">
         <v>6</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="20">
         <v>25</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="9">
         <v>7</v>
       </c>
-      <c r="D18" s="16">
-        <v>1</v>
-      </c>
-      <c r="E18" s="29">
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21">
         <v>50</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="22">
         <v>0.79800000000000004</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="9">
         <v>0.85299999999999998</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="9">
         <v>0.72199999999999998</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="10">
         <v>0.78200000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>7</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="3">
         <v>25</v>
       </c>
       <c r="C19" s="1">
@@ -1528,10 +1901,10 @@
       <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>50</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="4">
         <v>0.79400000000000004</v>
       </c>
       <c r="G19" s="1">
@@ -1545,31 +1918,31 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="31">
+      <c r="A20" s="23">
         <v>8</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="24">
         <v>25</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="11">
         <v>6</v>
       </c>
-      <c r="D20" s="20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="33">
+      <c r="D20" s="12">
+        <v>1</v>
+      </c>
+      <c r="E20" s="25">
         <v>200</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="26">
         <v>0.79800000000000004</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="11">
         <v>0.85199999999999998</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="11">
         <v>0.72299999999999998</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="12">
         <v>0.78200000000000003</v>
       </c>
     </row>
@@ -1968,4 +2341,2717 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDDC830-477D-4B66-B9EB-73083AA39AA2}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="7">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="1">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="9">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="11">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="47"/>
+      <c r="B11" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14">
+        <v>10</v>
+      </c>
+      <c r="C12" s="15">
+        <v>8</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17">
+        <v>100</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0.76</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>50</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>2</v>
+      </c>
+      <c r="B14" s="20">
+        <v>20</v>
+      </c>
+      <c r="C14" s="9">
+        <v>10</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21">
+        <v>50</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.78249999999999997</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>100</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>4</v>
+      </c>
+      <c r="B16" s="20">
+        <v>20</v>
+      </c>
+      <c r="C16" s="9">
+        <v>6</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21">
+        <v>50</v>
+      </c>
+      <c r="F16" s="22">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>50</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>6</v>
+      </c>
+      <c r="B18" s="20">
+        <v>25</v>
+      </c>
+      <c r="C18" s="9">
+        <v>7</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21">
+        <v>50</v>
+      </c>
+      <c r="F18" s="22">
+        <v>0.81</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.79</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>50</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="23">
+        <v>8</v>
+      </c>
+      <c r="B20" s="24">
+        <v>25</v>
+      </c>
+      <c r="C20" s="11">
+        <v>6</v>
+      </c>
+      <c r="D20" s="12">
+        <v>1</v>
+      </c>
+      <c r="E20" s="25">
+        <v>200</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0.81</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0.81699999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <v>300</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.78769999999999996</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.81699999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23">
+        <v>10</v>
+      </c>
+      <c r="B22" s="24">
+        <v>28</v>
+      </c>
+      <c r="C22" s="11">
+        <v>6</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="25">
+        <v>800</v>
+      </c>
+      <c r="F22" s="26">
+        <v>81</v>
+      </c>
+      <c r="G22" s="11">
+        <v>78.77</v>
+      </c>
+      <c r="H22" s="11">
+        <v>84.99</v>
+      </c>
+      <c r="I22" s="12">
+        <v>81.760000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>50</v>
+      </c>
+      <c r="F23" s="4">
+        <v>80.91</v>
+      </c>
+      <c r="G23" s="1">
+        <v>78.75</v>
+      </c>
+      <c r="H23" s="1">
+        <v>84.78</v>
+      </c>
+      <c r="I23" s="2">
+        <v>81.66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="23">
+        <v>12</v>
+      </c>
+      <c r="B24" s="24">
+        <v>15</v>
+      </c>
+      <c r="C24" s="11">
+        <v>4</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="25">
+        <v>50</v>
+      </c>
+      <c r="F24" s="26">
+        <v>80.66</v>
+      </c>
+      <c r="G24" s="11">
+        <v>85.13</v>
+      </c>
+      <c r="H24" s="11">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="I24" s="12">
+        <v>79.41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <v>50</v>
+      </c>
+      <c r="F25" s="4">
+        <v>76.61</v>
+      </c>
+      <c r="G25" s="1">
+        <v>80.56</v>
+      </c>
+      <c r="H25" s="1">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="I25" s="2">
+        <v>75.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="23">
+        <v>14</v>
+      </c>
+      <c r="B26" s="24">
+        <v>19</v>
+      </c>
+      <c r="C26" s="11">
+        <v>6</v>
+      </c>
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="25">
+        <v>500</v>
+      </c>
+      <c r="F26" s="26">
+        <v>81.03</v>
+      </c>
+      <c r="G26" s="11">
+        <v>78.81</v>
+      </c>
+      <c r="H26" s="11">
+        <v>84.99</v>
+      </c>
+      <c r="I26" s="12">
+        <v>81.78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>15</v>
+      </c>
+      <c r="B27" s="3">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>500</v>
+      </c>
+      <c r="F27" s="4">
+        <v>81</v>
+      </c>
+      <c r="G27" s="1">
+        <v>79.02</v>
+      </c>
+      <c r="H27" s="1">
+        <v>84.52</v>
+      </c>
+      <c r="I27" s="2">
+        <v>81.680000000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="23">
+        <v>16</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEB6269-607D-4AE1-8C7F-B80D834B86D0}">
+  <dimension ref="A1:Q27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="7">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.751</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="1">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="9">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="11">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="45"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="H12" s="1">
+        <v>78.8</v>
+      </c>
+      <c r="I12" s="1">
+        <v>82.33</v>
+      </c>
+      <c r="J12" s="2">
+        <v>80.52</v>
+      </c>
+      <c r="K12" s="4">
+        <v>80.3</v>
+      </c>
+      <c r="L12" s="1">
+        <v>78.790000000000006</v>
+      </c>
+      <c r="M12" s="1">
+        <v>83.02</v>
+      </c>
+      <c r="N12" s="2">
+        <v>80.849999999999994</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>2</v>
+      </c>
+      <c r="B13" s="20">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9">
+        <v>8</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21">
+        <v>5</v>
+      </c>
+      <c r="F13" s="21">
+        <v>5</v>
+      </c>
+      <c r="G13" s="22">
+        <v>79.98</v>
+      </c>
+      <c r="H13" s="9">
+        <v>79.209999999999994</v>
+      </c>
+      <c r="I13" s="9">
+        <v>81.28</v>
+      </c>
+      <c r="J13" s="10">
+        <v>80.23</v>
+      </c>
+      <c r="K13" s="22">
+        <v>80.27</v>
+      </c>
+      <c r="L13" s="9">
+        <v>79.069999999999993</v>
+      </c>
+      <c r="M13" s="9">
+        <v>82.43</v>
+      </c>
+      <c r="N13" s="10">
+        <v>80.72</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4">
+        <v>80.27</v>
+      </c>
+      <c r="H14" s="1">
+        <v>78.95</v>
+      </c>
+      <c r="I14" s="1">
+        <v>82.51</v>
+      </c>
+      <c r="J14" s="2">
+        <v>80.69</v>
+      </c>
+      <c r="K14" s="4">
+        <v>80.88</v>
+      </c>
+      <c r="L14" s="1">
+        <v>79.319999999999993</v>
+      </c>
+      <c r="M14" s="1">
+        <v>83.67</v>
+      </c>
+      <c r="N14" s="2">
+        <v>81.430000000000007</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20">
+        <v>20</v>
+      </c>
+      <c r="C15" s="9">
+        <v>8</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="21">
+        <v>5</v>
+      </c>
+      <c r="F15" s="21">
+        <v>5</v>
+      </c>
+      <c r="G15" s="22">
+        <v>78.61</v>
+      </c>
+      <c r="H15" s="9">
+        <v>77.790000000000006</v>
+      </c>
+      <c r="I15" s="9">
+        <v>80.05</v>
+      </c>
+      <c r="J15" s="10">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="K15" s="22">
+        <v>78.78</v>
+      </c>
+      <c r="L15" s="9">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="M15" s="9">
+        <v>81.06</v>
+      </c>
+      <c r="N15" s="10">
+        <v>79.290000000000006</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4</v>
+      </c>
+      <c r="G16" s="4">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="H16" s="1">
+        <v>78.39</v>
+      </c>
+      <c r="I16" s="1">
+        <v>80.06</v>
+      </c>
+      <c r="J16" s="2">
+        <v>79.22</v>
+      </c>
+      <c r="K16" s="4">
+        <v>79.209999999999994</v>
+      </c>
+      <c r="L16" s="1">
+        <v>78.31</v>
+      </c>
+      <c r="M16" s="1">
+        <v>80.91</v>
+      </c>
+      <c r="N16" s="2">
+        <v>79.59</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
+        <v>6</v>
+      </c>
+      <c r="B17" s="20">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9">
+        <v>8</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="21">
+        <v>5</v>
+      </c>
+      <c r="F17" s="21">
+        <v>10</v>
+      </c>
+      <c r="G17" s="22">
+        <v>79.73</v>
+      </c>
+      <c r="H17" s="9">
+        <v>79.08</v>
+      </c>
+      <c r="I17" s="9">
+        <v>80.84</v>
+      </c>
+      <c r="J17" s="10">
+        <v>79.95</v>
+      </c>
+      <c r="K17" s="22">
+        <v>79.94</v>
+      </c>
+      <c r="L17" s="9">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="M17" s="9">
+        <v>81.67</v>
+      </c>
+      <c r="N17" s="10">
+        <v>80.319999999999993</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5">
+        <v>4</v>
+      </c>
+      <c r="G18" s="4">
+        <v>79.67</v>
+      </c>
+      <c r="H18" s="1">
+        <v>78.92</v>
+      </c>
+      <c r="I18" s="1">
+        <v>80.95</v>
+      </c>
+      <c r="J18" s="2">
+        <v>79.92</v>
+      </c>
+      <c r="K18" s="4">
+        <v>80.12</v>
+      </c>
+      <c r="L18" s="1">
+        <v>78.98</v>
+      </c>
+      <c r="M18" s="1">
+        <v>82.2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>80.56</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="23">
+        <v>8</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="23">
+        <v>10</v>
+      </c>
+      <c r="B21" s="24">
+        <v>25</v>
+      </c>
+      <c r="C21" s="11">
+        <v>6</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="25">
+        <v>200</v>
+      </c>
+      <c r="F21" s="25">
+        <v>5</v>
+      </c>
+      <c r="G21" s="26"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>200</v>
+      </c>
+      <c r="F22" s="5">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="23">
+        <v>12</v>
+      </c>
+      <c r="B23" s="24">
+        <v>25</v>
+      </c>
+      <c r="C23" s="11">
+        <v>6</v>
+      </c>
+      <c r="D23" s="12">
+        <v>1</v>
+      </c>
+      <c r="E23" s="25">
+        <v>200</v>
+      </c>
+      <c r="F23" s="25">
+        <v>15</v>
+      </c>
+      <c r="G23" s="26"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>13</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="23">
+        <v>14</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="23">
+        <v>16</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C432B3-865D-4685-AF4A-CEBBD722EFF7}">
+  <dimension ref="A1:Q28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="58"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="74"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="85"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="88">
+        <v>76.64</v>
+      </c>
+      <c r="H4" s="89">
+        <v>80.790000000000006</v>
+      </c>
+      <c r="I4" s="89">
+        <v>69.88</v>
+      </c>
+      <c r="J4" s="90">
+        <v>74.94</v>
+      </c>
+      <c r="K4" s="91">
+        <v>76.77</v>
+      </c>
+      <c r="L4" s="89">
+        <v>81.09</v>
+      </c>
+      <c r="M4" s="89">
+        <v>69.94</v>
+      </c>
+      <c r="N4" s="90">
+        <v>75.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="92">
+        <v>80.91</v>
+      </c>
+      <c r="H5" s="93">
+        <v>79.180000000000007</v>
+      </c>
+      <c r="I5" s="93">
+        <v>83.86</v>
+      </c>
+      <c r="J5" s="94">
+        <v>81.45</v>
+      </c>
+      <c r="K5" s="95">
+        <v>80.87</v>
+      </c>
+      <c r="L5" s="93">
+        <v>78.8</v>
+      </c>
+      <c r="M5" s="93">
+        <v>84.57</v>
+      </c>
+      <c r="N5" s="94">
+        <v>81.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="96">
+        <v>80.91</v>
+      </c>
+      <c r="H6" s="97">
+        <v>79.06</v>
+      </c>
+      <c r="I6" s="97">
+        <v>84.07</v>
+      </c>
+      <c r="J6" s="98">
+        <v>81.489999999999995</v>
+      </c>
+      <c r="K6" s="99">
+        <v>80.91</v>
+      </c>
+      <c r="L6" s="97">
+        <v>78.64</v>
+      </c>
+      <c r="M6" s="97">
+        <v>84.99</v>
+      </c>
+      <c r="N6" s="98">
+        <v>81.69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="92">
+        <v>80.64</v>
+      </c>
+      <c r="H7" s="93">
+        <v>79.14</v>
+      </c>
+      <c r="I7" s="93">
+        <v>83.2</v>
+      </c>
+      <c r="J7" s="94">
+        <v>81.12</v>
+      </c>
+      <c r="K7" s="95">
+        <v>81.05</v>
+      </c>
+      <c r="L7" s="93">
+        <v>79.25</v>
+      </c>
+      <c r="M7" s="93">
+        <v>84.22</v>
+      </c>
+      <c r="N7" s="94">
+        <v>81.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="96">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="H8" s="97">
+        <v>79.13</v>
+      </c>
+      <c r="I8" s="97">
+        <v>83.9</v>
+      </c>
+      <c r="J8" s="98">
+        <v>81.45</v>
+      </c>
+      <c r="K8" s="99">
+        <v>81.13</v>
+      </c>
+      <c r="L8" s="97">
+        <v>79.040000000000006</v>
+      </c>
+      <c r="M8" s="97">
+        <v>84.84</v>
+      </c>
+      <c r="N8" s="98">
+        <v>81.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="77"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="47"/>
+      <c r="B12" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="H13" s="1">
+        <v>78.8</v>
+      </c>
+      <c r="I13" s="1">
+        <v>82.33</v>
+      </c>
+      <c r="J13" s="2">
+        <v>80.52</v>
+      </c>
+      <c r="K13" s="4">
+        <v>80.3</v>
+      </c>
+      <c r="L13" s="1">
+        <v>78.790000000000006</v>
+      </c>
+      <c r="M13" s="1">
+        <v>83.02</v>
+      </c>
+      <c r="N13" s="2">
+        <v>80.849999999999994</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>2</v>
+      </c>
+      <c r="B14" s="20">
+        <v>20</v>
+      </c>
+      <c r="C14" s="9">
+        <v>8</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21">
+        <v>5</v>
+      </c>
+      <c r="F14" s="21">
+        <v>5</v>
+      </c>
+      <c r="G14" s="22">
+        <v>79.98</v>
+      </c>
+      <c r="H14" s="9">
+        <v>79.209999999999994</v>
+      </c>
+      <c r="I14" s="9">
+        <v>81.28</v>
+      </c>
+      <c r="J14" s="10">
+        <v>80.23</v>
+      </c>
+      <c r="K14" s="22">
+        <v>80.27</v>
+      </c>
+      <c r="L14" s="9">
+        <v>79.069999999999993</v>
+      </c>
+      <c r="M14" s="9">
+        <v>82.43</v>
+      </c>
+      <c r="N14" s="10">
+        <v>80.72</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5">
+        <v>4</v>
+      </c>
+      <c r="G15" s="4">
+        <v>80.27</v>
+      </c>
+      <c r="H15" s="1">
+        <v>78.95</v>
+      </c>
+      <c r="I15" s="1">
+        <v>82.51</v>
+      </c>
+      <c r="J15" s="2">
+        <v>80.69</v>
+      </c>
+      <c r="K15" s="4">
+        <v>80.88</v>
+      </c>
+      <c r="L15" s="1">
+        <v>79.319999999999993</v>
+      </c>
+      <c r="M15" s="1">
+        <v>83.67</v>
+      </c>
+      <c r="N15" s="2">
+        <v>81.430000000000007</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>4</v>
+      </c>
+      <c r="B16" s="20">
+        <v>20</v>
+      </c>
+      <c r="C16" s="9">
+        <v>8</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21">
+        <v>5</v>
+      </c>
+      <c r="F16" s="21">
+        <v>5</v>
+      </c>
+      <c r="G16" s="22">
+        <v>78.61</v>
+      </c>
+      <c r="H16" s="9">
+        <v>77.790000000000006</v>
+      </c>
+      <c r="I16" s="9">
+        <v>80.05</v>
+      </c>
+      <c r="J16" s="10">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="K16" s="22">
+        <v>78.78</v>
+      </c>
+      <c r="L16" s="9">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="M16" s="9">
+        <v>81.06</v>
+      </c>
+      <c r="N16" s="10">
+        <v>79.290000000000006</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4</v>
+      </c>
+      <c r="G17" s="4">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="H17" s="1">
+        <v>78.39</v>
+      </c>
+      <c r="I17" s="1">
+        <v>80.06</v>
+      </c>
+      <c r="J17" s="2">
+        <v>79.22</v>
+      </c>
+      <c r="K17" s="4">
+        <v>79.209999999999994</v>
+      </c>
+      <c r="L17" s="1">
+        <v>78.31</v>
+      </c>
+      <c r="M17" s="1">
+        <v>80.91</v>
+      </c>
+      <c r="N17" s="2">
+        <v>79.59</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>6</v>
+      </c>
+      <c r="B18" s="20">
+        <v>20</v>
+      </c>
+      <c r="C18" s="9">
+        <v>8</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21">
+        <v>5</v>
+      </c>
+      <c r="F18" s="21">
+        <v>10</v>
+      </c>
+      <c r="G18" s="22">
+        <v>79.73</v>
+      </c>
+      <c r="H18" s="9">
+        <v>79.08</v>
+      </c>
+      <c r="I18" s="9">
+        <v>80.84</v>
+      </c>
+      <c r="J18" s="10">
+        <v>79.95</v>
+      </c>
+      <c r="K18" s="22">
+        <v>79.94</v>
+      </c>
+      <c r="L18" s="9">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="M18" s="9">
+        <v>81.67</v>
+      </c>
+      <c r="N18" s="10">
+        <v>80.319999999999993</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5">
+        <v>4</v>
+      </c>
+      <c r="G19" s="4">
+        <v>79.67</v>
+      </c>
+      <c r="H19" s="1">
+        <v>78.92</v>
+      </c>
+      <c r="I19" s="1">
+        <v>80.95</v>
+      </c>
+      <c r="J19" s="2">
+        <v>79.92</v>
+      </c>
+      <c r="K19" s="4">
+        <v>80.12</v>
+      </c>
+      <c r="L19" s="1">
+        <v>78.98</v>
+      </c>
+      <c r="M19" s="1">
+        <v>82.2</v>
+      </c>
+      <c r="N19" s="2">
+        <v>80.56</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="23">
+        <v>8</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23">
+        <v>10</v>
+      </c>
+      <c r="B22" s="24">
+        <v>25</v>
+      </c>
+      <c r="C22" s="11">
+        <v>6</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="25">
+        <v>200</v>
+      </c>
+      <c r="F22" s="25">
+        <v>5</v>
+      </c>
+      <c r="G22" s="26">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="H22" s="11">
+        <v>79.13</v>
+      </c>
+      <c r="I22" s="11">
+        <v>83.9</v>
+      </c>
+      <c r="J22" s="12">
+        <v>81.45</v>
+      </c>
+      <c r="K22" s="26">
+        <v>81.13</v>
+      </c>
+      <c r="L22" s="11">
+        <v>79.040000000000006</v>
+      </c>
+      <c r="M22" s="11">
+        <v>84.84</v>
+      </c>
+      <c r="N22" s="12">
+        <v>81.84</v>
+      </c>
+      <c r="O22" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>200</v>
+      </c>
+      <c r="F23" s="5">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4">
+        <v>80.86</v>
+      </c>
+      <c r="H23" s="1">
+        <v>79.06</v>
+      </c>
+      <c r="I23" s="1">
+        <v>83.94</v>
+      </c>
+      <c r="J23" s="2">
+        <v>81.430000000000007</v>
+      </c>
+      <c r="K23" s="4">
+        <v>80.94</v>
+      </c>
+      <c r="L23" s="1">
+        <v>78.84</v>
+      </c>
+      <c r="M23" s="1">
+        <v>84.69</v>
+      </c>
+      <c r="N23" s="2">
+        <v>81.66</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="23">
+        <v>12</v>
+      </c>
+      <c r="B24" s="24">
+        <v>25</v>
+      </c>
+      <c r="C24" s="11">
+        <v>6</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="25">
+        <v>200</v>
+      </c>
+      <c r="F24" s="25">
+        <v>15</v>
+      </c>
+      <c r="G24" s="26">
+        <v>80.88</v>
+      </c>
+      <c r="H24" s="11">
+        <v>79.17</v>
+      </c>
+      <c r="I24" s="11">
+        <v>83.78</v>
+      </c>
+      <c r="J24" s="12">
+        <v>81.41</v>
+      </c>
+      <c r="K24" s="26">
+        <v>81.06</v>
+      </c>
+      <c r="L24" s="11">
+        <v>79.11</v>
+      </c>
+      <c r="M24" s="11">
+        <v>84.52</v>
+      </c>
+      <c r="N24" s="12">
+        <v>81.72</v>
+      </c>
+      <c r="O24" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="23">
+        <v>14</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>15</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="23">
+        <v>16</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A10:Q10"/>
+    <mergeCell ref="A2:F3"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="G2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>